<commit_message>
updated event data flow table
</commit_message>
<xml_diff>
--- a/docs/Event-Data-Flow-Table.xlsx
+++ b/docs/Event-Data-Flow-Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasgleiter/dev/src/tobiasgleiter/github/nextjs13-mqtt-microservices/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE07E66-CB98-E84E-8E40-59362E7085ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF79E5-8D1D-EE4A-8F74-CA3365310578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" xr2:uid="{7C259524-F72C-3A4D-B8C1-8881A94EDEA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Entity ID</t>
   </si>
@@ -125,15 +125,6 @@
     <t>{ id: xx, { id: yy, content: bla bla, status: "rejected"}}</t>
   </si>
   <si>
-    <t>query</t>
-  </si>
-  <si>
-    <t>query/all</t>
-  </si>
-  <si>
-    <t>[{}, {}, {}, ….]</t>
-  </si>
-  <si>
     <t>Create new post</t>
   </si>
   <si>
@@ -156,15 +147,6 @@
   </si>
   <si>
     <t>Set Status of comment as rejected</t>
-  </si>
-  <si>
-    <t>query/one</t>
-  </si>
-  <si>
-    <t>Get all posts with comments</t>
-  </si>
-  <si>
-    <t>Get one post by ID</t>
   </si>
 </sst>
 </file>
@@ -553,7 +535,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +583,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -621,7 +603,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -641,7 +623,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -669,7 +651,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -689,7 +671,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -709,7 +691,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -737,7 +719,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -757,7 +739,7 @@
         <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -769,44 +751,20 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>